<commit_message>
feat: export new table
</commit_message>
<xml_diff>
--- a/formatExcel/DB/Proyectos_Unicos.xlsx
+++ b/formatExcel/DB/Proyectos_Unicos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wilson/Desktop/DB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wilson/PhpstormProjects/plannerapp/formatExcel/DB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{974B6C98-2549-5648-AA8C-18D34CE32F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6672037-CB4D-DA45-8EB3-C0B36088398D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{56D05D2C-E0BB-7543-AAC5-D25C0EEA2D55}"/>
   </bookViews>
@@ -566,7 +566,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="A2" sqref="A2:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>